<commit_message>
sequence, correction, class, gantt, deployment
</commit_message>
<xml_diff>
--- a/DD/gantt/gantt.xlsx
+++ b/DD/gantt/gantt.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matteo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matteo\Desktop\progetto software engineering 2\MoscatelliPozzoli\DD\gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="39">
   <si>
     <t>Project Plan</t>
   </si>
@@ -92,12 +92,6 @@
     <t>Second Phase Testing</t>
   </si>
   <si>
-    <t>StatisticHandler Implementation</t>
-  </si>
-  <si>
-    <t>StatisticHandler, DataBaseHandler Integration</t>
-  </si>
-  <si>
     <t>AuthorityHandler, EndUserHandler, StatisticHandler Integration</t>
   </si>
   <si>
@@ -132,6 +126,21 @@
   </si>
   <si>
     <t>Fourth Phase Testing</t>
+  </si>
+  <si>
+    <t>StatisticsHandler Implementation</t>
+  </si>
+  <si>
+    <t>StatisticsHandler, DataBaseHandler Integration</t>
+  </si>
+  <si>
+    <t>AuthorityHandler, EndUserHandler, StatisticsHandler Integration</t>
+  </si>
+  <si>
+    <t>StatisticsHandler and Map services integration</t>
+  </si>
+  <si>
+    <t>StatisticsHandler, MunicipalityHandler, DataBaseHandler Integration</t>
   </si>
 </sst>
 </file>
@@ -946,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:S60"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1635,7 +1644,7 @@
     </row>
     <row r="35" spans="1:23" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="47" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B35" s="48">
         <v>2</v>
@@ -1821,7 +1830,7 @@
     </row>
     <row r="41" spans="1:23" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="47" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B41" s="48">
         <v>7</v>
@@ -1852,7 +1861,7 @@
     </row>
     <row r="42" spans="1:23" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="47" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B42" s="48">
         <v>7</v>
@@ -1883,7 +1892,7 @@
     </row>
     <row r="43" spans="1:23" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="47" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B43" s="48">
         <v>7</v>
@@ -1914,7 +1923,7 @@
     </row>
     <row r="44" spans="1:23" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="47" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B44" s="48">
         <v>10</v>
@@ -1945,7 +1954,7 @@
     </row>
     <row r="45" spans="1:23" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="47" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B45" s="48">
         <v>10</v>
@@ -1976,7 +1985,7 @@
     </row>
     <row r="46" spans="1:23" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="47" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B46" s="48">
         <v>12</v>
@@ -2008,7 +2017,7 @@
     <row r="47" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="1:23" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="50" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
@@ -2145,7 +2154,7 @@
     </row>
     <row r="54" spans="1:23" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="47" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B54" s="48">
         <v>3</v>
@@ -2176,7 +2185,7 @@
     </row>
     <row r="55" spans="1:23" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="47" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B55" s="48">
         <v>2</v>
@@ -2238,7 +2247,7 @@
     </row>
     <row r="57" spans="1:23" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="47" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B57" s="48">
         <v>7</v>
@@ -2269,7 +2278,7 @@
     </row>
     <row r="58" spans="1:23" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="47" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B58" s="48">
         <v>7</v>
@@ -2300,7 +2309,7 @@
     </row>
     <row r="59" spans="1:23" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="47" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B59" s="48">
         <v>9</v>
@@ -2331,7 +2340,7 @@
     </row>
     <row r="60" spans="1:23" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="47" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B60" s="48">
         <v>12</v>

</xml_diff>